<commit_message>
most recent models & outputs
</commit_message>
<xml_diff>
--- a/Gantt Lake Stable Isotope/Gantt_MixSIAR Outputs.xlsx
+++ b/Gantt Lake Stable Isotope/Gantt_MixSIAR Outputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjf0021\Documents\GitHub\Gantt-Stable-Isotope\Gantt Lake Stable Isotope\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{429AFC63-A6FA-44FE-B43B-1AAE83415C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D2C923-42B0-4FB8-AE04-233860675691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1575" windowWidth="29040" windowHeight="15840" xr2:uid="{8C96F04C-207B-8F44-AB27-8BF7B317D104}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="code" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
   <si>
     <t xml:space="preserve">NULL Model - Uninformative Prior </t>
   </si>
@@ -477,6 +476,9 @@
   </si>
   <si>
     <t>p.global.SPOM 0.012 0.011 0.000 0.001 0.004 0.009 0.017 0.035 0.041</t>
+  </si>
+  <si>
+    <t>Species Model</t>
   </si>
 </sst>
 </file>
@@ -837,75 +839,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB8568C-D1DF-4FAA-B5AC-3428BEBAF4C2}">
-  <dimension ref="A1:A46"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>131</v>
       </c>

</xml_diff>